<commit_message>
Vrwondplus, extended macros for hwwi/hwwz; wordsunknowntoalpino lexicon
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D43CC8-38FB-42B9-B54A-6B57763390B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11072BB-6618-4A70-929A-7AF351BF7237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1647,13 +1647,6 @@
     node[(@pt="n"  or (@pt="adj" and @positie="nom")) and @rel="hd"]]</t>
   </si>
   <si>
-    <t>//node[(((@cat="sv1" and not(parent::node[@cat="whq"])) or
-        (@cat="smain" )
-       ) and 
-  node[@pt="ww" and @rel="hd" and (not(@stype) or @stype!="imparative") ] and node[@rel="su" and number(@end)&gt;../node[@rel="hd"]/@end]) or 
-  %robustinversion%]</t>
-  </si>
-  <si>
     <t>//node[node[@pt="ww"  and @rel ="hd"] and node[@rel="pc" and not(%Tarsp_B%)]]</t>
   </si>
   <si>
@@ -1827,9 +1820,6 @@
     <t>//node[(@lemma="hij" or @lemma="ie")  and @pt="vnw"]</t>
   </si>
   <si>
-    <t>//node[@cat="whq" and node[@cat="sv1"] and count(node)=1]</t>
-  </si>
-  <si>
     <t>//node[(@pt="ww" and @rel="hd" and 
            (@lemma="hebben" or @lemma="worden" or @lemma="zijn") and
        parent::node[node[@rel="vc" and ((@cat="ppart" and node[@rel="hd"]) or (@pt="ww" and @wvorm="vd"))]
@@ -1923,6 +1913,20 @@
   </si>
   <si>
     <t>G_Zn</t>
+  </si>
+  <si>
+    <t>//node[%vrwondplus%]</t>
+  </si>
+  <si>
+    <t>//node[
+(
+ (
+  (@cat="sv1" and not(parent::node[@cat="whq"])) or
+  (@cat="smain" )
+ ) and 
+  node[@pt="ww" and @rel="hd" and (not(@stype) or @stype!="imparative") ] and node[@rel="su" and number(@end)&gt;../node[@rel="hd"]/@end]
+) or 
+%robustinversion%]</t>
   </si>
 </sst>
 </file>
@@ -2343,11 +2347,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F139" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G39" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="F141" sqref="F141"/>
+      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2411,22 +2415,22 @@
         <v>448</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>575</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2446,13 +2450,13 @@
         <v>197</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>358</v>
@@ -2464,7 +2468,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>569</v>
+        <v>598</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>358</v>
@@ -2558,7 +2562,7 @@
         <v>449</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2622,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>358</v>
@@ -2651,7 +2655,7 @@
         <v>197</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>358</v>
@@ -2841,7 +2845,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>358</v>
@@ -2853,7 +2857,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>358</v>
@@ -3089,7 +3093,7 @@
         <v>396</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>358</v>
@@ -3101,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>358</v>
@@ -3232,7 +3236,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>358</v>
@@ -3244,7 +3248,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>358</v>
@@ -3276,7 +3280,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>358</v>
@@ -3288,7 +3292,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>358</v>
@@ -3504,7 +3508,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>358</v>
@@ -3656,7 +3660,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>358</v>
@@ -3761,7 +3765,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>358</v>
@@ -3790,7 +3794,7 @@
         <v>214</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>358</v>
@@ -3802,7 +3806,7 @@
         <v>368</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>358</v>
@@ -3831,7 +3835,7 @@
         <v>215</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>358</v>
@@ -3843,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>358</v>
@@ -3869,7 +3873,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>358</v>
@@ -3972,7 +3976,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>259</v>
       </c>
@@ -4001,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>519</v>
+        <v>599</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>358</v>
@@ -4106,7 +4110,7 @@
         <v>207</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>358</v>
@@ -4182,7 +4186,7 @@
         <v>359</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>359</v>
@@ -4480,7 +4484,7 @@
         <v>449</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4506,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>359</v>
@@ -4535,7 +4539,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>358</v>
@@ -4547,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>358</v>
@@ -4576,7 +4580,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>358</v>
@@ -4588,7 +4592,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>358</v>
@@ -4638,7 +4642,7 @@
         <v>449</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4819,7 +4823,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>358</v>
@@ -4848,7 +4852,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>358</v>
@@ -4860,7 +4864,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>358</v>
@@ -4889,7 +4893,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>358</v>
@@ -4901,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>358</v>
@@ -4930,7 +4934,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>358</v>
@@ -4971,7 +4975,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>358</v>
@@ -5012,7 +5016,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>358</v>
@@ -5024,7 +5028,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>358</v>
@@ -5053,7 +5057,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>358</v>
@@ -5065,7 +5069,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>358</v>
@@ -5094,10 +5098,10 @@
         <v>412</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>358</v>
@@ -5135,10 +5139,10 @@
         <v>192</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>358</v>
@@ -5150,7 +5154,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>358</v>
@@ -5200,7 +5204,7 @@
         <v>449</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5235,7 +5239,7 @@
         <v>449</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5293,10 +5297,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>358</v>
@@ -5308,7 +5312,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>358</v>
@@ -5337,10 +5341,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>358</v>
@@ -5352,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>358</v>
@@ -5378,7 +5382,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>358</v>
@@ -5463,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>358</v>
@@ -5577,7 +5581,7 @@
         <v>449</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5702,7 +5706,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>358</v>
@@ -5836,7 +5840,7 @@
         <v>358</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>359</v>
@@ -5877,7 +5881,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>358</v>
@@ -5906,7 +5910,7 @@
         <v>24</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>358</v>
@@ -5947,7 +5951,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>358</v>
@@ -5959,7 +5963,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>358</v>
@@ -6026,7 +6030,7 @@
         <v>458</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>358</v>
@@ -6070,7 +6074,7 @@
         <v>449</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6175,7 +6179,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>358</v>
@@ -6210,7 +6214,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>358</v>
@@ -6298,7 +6302,7 @@
         <v>461</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>170</v>
@@ -6362,7 +6366,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>358</v>
@@ -6403,7 +6407,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>358</v>
@@ -6444,7 +6448,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>358</v>
@@ -6530,7 +6534,7 @@
         <v>449</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6556,7 +6560,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>358</v>
@@ -6592,7 +6596,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>358</v>
@@ -6653,7 +6657,7 @@
         <v>197</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>358</v>
@@ -6665,7 +6669,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>359</v>
@@ -6700,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>358</v>
@@ -6732,7 +6736,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>358</v>
@@ -6864,7 +6868,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>358</v>
@@ -6876,7 +6880,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>358</v>
@@ -7010,7 +7014,7 @@
         <v>71</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>358</v>
@@ -7022,7 +7026,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>358</v>
@@ -7051,7 +7055,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>358</v>
@@ -7063,7 +7067,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>358</v>
@@ -7095,7 +7099,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>358</v>
@@ -7107,7 +7111,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>358</v>
@@ -7177,7 +7181,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>358</v>
@@ -7238,7 +7242,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>358</v>
@@ -7250,7 +7254,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>358</v>
@@ -7279,7 +7283,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>358</v>
@@ -7291,7 +7295,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>358</v>
@@ -7323,7 +7327,7 @@
         <v>447</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>358</v>
@@ -7335,7 +7339,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>358</v>
@@ -7448,7 +7452,7 @@
         <v>209</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>358</v>
@@ -7612,7 +7616,7 @@
         <v>449</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -7629,7 +7633,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>358</v>
@@ -7641,7 +7645,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>358</v>
@@ -7906,7 +7910,7 @@
         <v>416</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>358</v>
@@ -8087,7 +8091,7 @@
         <v>450</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Various updates Hwwi, HwwZ, OndW, VUDiv, kijk intermediate commit
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11072BB-6618-4A70-929A-7AF351BF7237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F608D15-6F7A-4381-BD6B-C0188FD7324D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="601">
   <si>
     <t>Item</t>
   </si>
@@ -1927,6 +1927,9 @@
   node[@pt="ww" and @rel="hd" and (not(@stype) or @stype!="imparative") ] and node[@rel="su" and number(@end)&gt;../node[@rel="hd"]/@end]
 ) or 
 %robustinversion%]</t>
+  </si>
+  <si>
+    <t>//node[%Tarsp_vcw%]</t>
   </si>
 </sst>
 </file>
@@ -2347,11 +2350,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G88" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
+      <selection pane="bottomRight" activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5921,6 +5924,9 @@
       <c r="J94" s="2">
         <v>2</v>
       </c>
+      <c r="K94" s="2" t="s">
+        <v>600</v>
+      </c>
       <c r="L94" s="2" t="s">
         <v>358</v>
       </c>

</xml_diff>

<commit_message>
Various updates: HwwZ, Hwwi, OndW, Stam
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F608D15-6F7A-4381-BD6B-C0188FD7324D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F3087-293C-42CB-9F2C-B725737045EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1595,13 +1595,6 @@
     <t>//node[%Tarsp_HwwZ%]</t>
   </si>
   <si>
-    <t>//node[@pt="ww" and @pvagr="met-t" and not(%Tarsp_hww% or
-     @lemma = "hebben" or
-     @lemma = "worden" or
-     @lemma = "zijn"   
-  ) ]</t>
-  </si>
-  <si>
     <t>//node[node[@rel="hd" and @pt="vz"] and 
        node[@rel="obj1" and 
             ( (@pt="vz" or @pt="bw") or 
@@ -1930,6 +1923,10 @@
   </si>
   <si>
     <t>//node[%Tarsp_vcw%]</t>
+  </si>
+  <si>
+    <t>//node[@pt="ww" and @pvagr="met-t" and 
+not(%Tarsp_hww% or %hebbenwordenzijn%  ) ]</t>
   </si>
 </sst>
 </file>
@@ -2350,11 +2347,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="H88" sqref="H88"/>
+      <selection pane="bottomRight" activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2418,22 +2415,22 @@
         <v>448</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>573</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2453,13 +2450,13 @@
         <v>197</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>358</v>
@@ -2471,7 +2468,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>358</v>
@@ -2565,7 +2562,7 @@
         <v>449</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2629,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>358</v>
@@ -2658,7 +2655,7 @@
         <v>197</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>358</v>
@@ -2670,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>359</v>
@@ -2784,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>358</v>
@@ -2848,7 +2845,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>358</v>
@@ -2860,7 +2857,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>358</v>
@@ -2968,7 +2965,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>358</v>
@@ -3096,7 +3093,7 @@
         <v>396</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>358</v>
@@ -3108,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>358</v>
@@ -3239,7 +3236,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>358</v>
@@ -3251,7 +3248,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>358</v>
@@ -3283,7 +3280,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>358</v>
@@ -3295,7 +3292,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>358</v>
@@ -3307,7 +3304,7 @@
         <v>449</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -3365,7 +3362,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>358</v>
@@ -3511,7 +3508,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>358</v>
@@ -3663,7 +3660,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>358</v>
@@ -3768,7 +3765,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>358</v>
@@ -3797,7 +3794,7 @@
         <v>214</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>358</v>
@@ -3809,7 +3806,7 @@
         <v>368</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>358</v>
@@ -3838,7 +3835,7 @@
         <v>215</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>358</v>
@@ -3850,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>358</v>
@@ -3876,7 +3873,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>358</v>
@@ -4008,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>358</v>
@@ -4046,7 +4043,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>358</v>
@@ -4113,7 +4110,7 @@
         <v>207</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>358</v>
@@ -4189,7 +4186,7 @@
         <v>359</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>359</v>
@@ -4487,7 +4484,7 @@
         <v>449</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4513,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>359</v>
@@ -4542,7 +4539,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>358</v>
@@ -4554,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>358</v>
@@ -4583,7 +4580,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>358</v>
@@ -4595,7 +4592,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>358</v>
@@ -4645,7 +4642,7 @@
         <v>449</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4826,7 +4823,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>358</v>
@@ -4855,7 +4852,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>358</v>
@@ -4867,7 +4864,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>358</v>
@@ -4896,7 +4893,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>358</v>
@@ -4908,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>358</v>
@@ -4937,7 +4934,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>358</v>
@@ -4978,7 +4975,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>358</v>
@@ -5019,7 +5016,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>358</v>
@@ -5031,7 +5028,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>358</v>
@@ -5060,7 +5057,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>358</v>
@@ -5072,7 +5069,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>358</v>
@@ -5101,10 +5098,10 @@
         <v>412</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>358</v>
@@ -5142,10 +5139,10 @@
         <v>192</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>358</v>
@@ -5157,7 +5154,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>358</v>
@@ -5207,7 +5204,7 @@
         <v>449</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5242,7 +5239,7 @@
         <v>449</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5300,10 +5297,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>358</v>
@@ -5315,7 +5312,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>358</v>
@@ -5344,10 +5341,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>358</v>
@@ -5359,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>358</v>
@@ -5385,7 +5382,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>358</v>
@@ -5470,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>358</v>
@@ -5482,7 +5479,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>298</v>
       </c>
@@ -5508,7 +5505,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>507</v>
+        <v>600</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>358</v>
@@ -5584,7 +5581,7 @@
         <v>449</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5697,7 +5694,7 @@
         <v>388</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>358</v>
@@ -5709,7 +5706,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>358</v>
@@ -5805,7 +5802,7 @@
         <v>389</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>358</v>
@@ -5843,7 +5840,7 @@
         <v>358</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>359</v>
@@ -5884,7 +5881,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>358</v>
@@ -5913,7 +5910,7 @@
         <v>24</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>358</v>
@@ -5925,7 +5922,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>358</v>
@@ -5957,7 +5954,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>358</v>
@@ -5969,7 +5966,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>358</v>
@@ -6036,7 +6033,7 @@
         <v>458</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>358</v>
@@ -6080,7 +6077,7 @@
         <v>449</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6185,7 +6182,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>358</v>
@@ -6220,7 +6217,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>358</v>
@@ -6308,7 +6305,7 @@
         <v>461</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>170</v>
@@ -6372,7 +6369,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>358</v>
@@ -6413,7 +6410,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>358</v>
@@ -6454,7 +6451,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>358</v>
@@ -6495,7 +6492,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>358</v>
@@ -6540,7 +6537,7 @@
         <v>449</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6566,7 +6563,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>358</v>
@@ -6602,7 +6599,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>358</v>
@@ -6663,7 +6660,7 @@
         <v>197</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>358</v>
@@ -6675,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>359</v>
@@ -6710,7 +6707,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>358</v>
@@ -6742,7 +6739,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>358</v>
@@ -6874,7 +6871,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>358</v>
@@ -6886,7 +6883,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>358</v>
@@ -7020,7 +7017,7 @@
         <v>71</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>358</v>
@@ -7032,7 +7029,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>358</v>
@@ -7061,7 +7058,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>358</v>
@@ -7073,7 +7070,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>358</v>
@@ -7105,7 +7102,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>358</v>
@@ -7117,7 +7114,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>358</v>
@@ -7187,7 +7184,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>358</v>
@@ -7248,7 +7245,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>358</v>
@@ -7260,7 +7257,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>358</v>
@@ -7289,7 +7286,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>358</v>
@@ -7301,7 +7298,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>358</v>
@@ -7333,7 +7330,7 @@
         <v>447</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>358</v>
@@ -7345,7 +7342,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>358</v>
@@ -7417,7 +7414,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>358</v>
@@ -7458,7 +7455,7 @@
         <v>209</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>358</v>
@@ -7499,7 +7496,7 @@
         <v>41</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>358</v>
@@ -7622,7 +7619,7 @@
         <v>449</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -7639,7 +7636,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>358</v>
@@ -7651,7 +7648,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>358</v>
@@ -7712,7 +7709,7 @@
         <v>198</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>358</v>
@@ -7916,7 +7913,7 @@
         <v>416</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>358</v>
@@ -8097,7 +8094,7 @@
         <v>450</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
First update of nominal + pastaprt small clauses
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD24FE2D-9D69-4E2E-A7D3-6235B636F867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471DC713-947D-4F6C-95F9-29E005A746E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="602">
   <si>
     <t>Item</t>
   </si>
@@ -1724,16 +1724,6 @@
          (@rel="--" or @rel="sat" or @rel="tag"))  		 
 		 ) )	or  %Tarsp_kijkVU%	 or %Tarsp_hehe%
 ]</t>
-  </si>
-  <si>
-    <t>//node[@pt="ww" and @pvtijd="tgw" and
-        not(%Tarsp_kijkVU%) and
- not(%Tarsp_hww% or
-     @lemma = "hebben" or
-     @lemma = "worden" or
-     @lemma = "zijn"   
-  )
-and @pvagr="ev"  ]</t>
   </si>
   <si>
     <t>//node[((@rel="vc" or @rel="su") and (@cat="cp" or @cat="whsub")) or %directerede_vcbijzin%]</t>
@@ -1914,12 +1904,26 @@
     <t>//node[%Tarsp_vcw%]</t>
   </si>
   <si>
-    <t>//node[@pt="ww" and @pvagr="met-t" and 
-not(%Tarsp_hww% or %hebbenwordenzijn%  ) ]</t>
-  </si>
-  <si>
     <t xml:space="preserve">//node[%inv%]
 </t>
+  </si>
+  <si>
+    <t>//node[@pt="ww" and @pvtijd="tgw" and
+        not(%Tarsp_kijkVU%) and not(%Tarsp_Kop%) and
+ not(%Tarsp_hww% or
+     @lemma = "hebben" or
+     @lemma = "worden" or
+     @lemma = "zijn"   
+  )
+and not(parent::node[%basicimperative%])
+and @pvagr="ev"  ]</t>
+  </si>
+  <si>
+    <t>//node[@pt="ww" and @pvagr="met-t" and not(%Tarsp_Kop%) and
+not(%Tarsp_hww% or %hebbenwordenzijn%  ) ]</t>
+  </si>
+  <si>
+    <t>99</t>
   </si>
 </sst>
 </file>
@@ -2340,11 +2344,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G48" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomRight" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2408,22 +2412,22 @@
         <v>448</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>572</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2443,13 +2447,13 @@
         <v>197</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>358</v>
@@ -2461,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>358</v>
@@ -2555,7 +2559,7 @@
         <v>449</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2619,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>358</v>
@@ -2648,7 +2652,7 @@
         <v>197</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>358</v>
@@ -2838,7 +2842,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>358</v>
@@ -3086,7 +3090,7 @@
         <v>396</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>358</v>
@@ -3098,7 +3102,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>358</v>
@@ -3229,7 +3233,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>358</v>
@@ -3273,7 +3277,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>358</v>
@@ -3285,7 +3289,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>358</v>
@@ -3501,7 +3505,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>358</v>
@@ -3653,7 +3657,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>358</v>
@@ -3758,7 +3762,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>358</v>
@@ -3787,7 +3791,7 @@
         <v>214</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>358</v>
@@ -3828,7 +3832,7 @@
         <v>215</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>358</v>
@@ -3840,7 +3844,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>358</v>
@@ -3866,7 +3870,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>358</v>
@@ -3998,7 +4002,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>358</v>
@@ -4103,7 +4107,7 @@
         <v>207</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>358</v>
@@ -4477,7 +4481,7 @@
         <v>449</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4503,7 +4507,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>359</v>
@@ -4532,7 +4536,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>358</v>
@@ -4544,7 +4548,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>358</v>
@@ -4573,7 +4577,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>358</v>
@@ -4585,7 +4589,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>358</v>
@@ -4635,7 +4639,7 @@
         <v>449</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4816,7 +4820,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>358</v>
@@ -4845,7 +4849,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>358</v>
@@ -4857,7 +4861,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>358</v>
@@ -4886,7 +4890,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>358</v>
@@ -4898,7 +4902,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>358</v>
@@ -4927,7 +4931,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>358</v>
@@ -4968,7 +4972,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>358</v>
@@ -5009,7 +5013,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>358</v>
@@ -5050,7 +5054,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>358</v>
@@ -5091,10 +5095,10 @@
         <v>412</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>358</v>
@@ -5132,10 +5136,10 @@
         <v>192</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>358</v>
@@ -5197,7 +5201,7 @@
         <v>449</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5232,7 +5236,7 @@
         <v>449</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5290,10 +5294,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>358</v>
@@ -5334,10 +5338,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>358</v>
@@ -5375,7 +5379,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>358</v>
@@ -5437,7 +5441,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>297</v>
       </c>
@@ -5451,7 +5455,7 @@
         <v>149</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>358</v>
+        <v>601</v>
       </c>
       <c r="I81" s="2">
         <v>86</v>
@@ -5460,7 +5464,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>543</v>
+        <v>599</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>358</v>
@@ -5472,7 +5476,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>298</v>
       </c>
@@ -5498,7 +5502,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>358</v>
@@ -5574,7 +5578,7 @@
         <v>449</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5874,7 +5878,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>358</v>
@@ -5903,7 +5907,7 @@
         <v>24</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>358</v>
@@ -5915,7 +5919,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>358</v>
@@ -5947,7 +5951,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>358</v>
@@ -6070,7 +6074,7 @@
         <v>449</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6175,7 +6179,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>358</v>
@@ -6210,7 +6214,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>358</v>
@@ -6298,7 +6302,7 @@
         <v>461</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>170</v>
@@ -6530,7 +6534,7 @@
         <v>449</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6556,7 +6560,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>358</v>
@@ -6592,7 +6596,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>358</v>
@@ -6653,7 +6657,7 @@
         <v>197</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>358</v>
@@ -6700,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>358</v>
@@ -6732,7 +6736,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>358</v>
@@ -6864,7 +6868,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>358</v>
@@ -7010,7 +7014,7 @@
         <v>71</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>358</v>
@@ -7051,7 +7055,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>358</v>
@@ -7095,7 +7099,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>358</v>
@@ -7238,7 +7242,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>358</v>
@@ -7279,7 +7283,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>358</v>
@@ -7323,7 +7327,7 @@
         <v>447</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>358</v>
@@ -7448,7 +7452,7 @@
         <v>209</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>358</v>
@@ -7612,7 +7616,7 @@
         <v>449</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -7629,7 +7633,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>358</v>
@@ -7641,7 +7645,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>358</v>
@@ -7906,7 +7910,7 @@
         <v>416</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>358</v>
@@ -8087,7 +8091,7 @@
         <v>450</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
First update of BX, OndVC and BBX
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5B343E-FB5F-4A3C-84AA-0F69B6D1E488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9064BBB-6D8B-4592-9AE8-58F4F389F530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1585,11 +1585,6 @@
               (%Rpronoun% and @begin=../node[@rel="hd"]/@end)) ]]</t>
   </si>
   <si>
-    <t>//node[(node[@rel="mod" and %adjoradv%] and
-       node[@rel="hd"  and %adjoradv%])     
-   ]</t>
-  </si>
-  <si>
     <t>vu nee/ja, vu ja/nee,V.U. Ja/nee, nee, ja</t>
   </si>
   <si>
@@ -1915,6 +1910,10 @@
   </si>
   <si>
     <t>//node[%Xneg%]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//node[%bbvb%]
+</t>
   </si>
 </sst>
 </file>
@@ -2335,11 +2334,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K136" sqref="K136"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2403,22 +2402,22 @@
         <v>445</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>566</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2438,13 +2437,13 @@
         <v>195</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>356</v>
@@ -2456,7 +2455,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>356</v>
@@ -2550,7 +2549,7 @@
         <v>446</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2614,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>356</v>
@@ -2643,7 +2642,7 @@
         <v>195</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>356</v>
@@ -2655,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>357</v>
@@ -2746,7 +2745,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>224</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>504</v>
+        <v>602</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>356</v>
@@ -2833,7 +2832,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>356</v>
@@ -2845,7 +2844,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>356</v>
@@ -2953,7 +2952,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>356</v>
@@ -3081,7 +3080,7 @@
         <v>393</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>356</v>
@@ -3093,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>356</v>
@@ -3224,7 +3223,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>356</v>
@@ -3236,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>356</v>
@@ -3268,7 +3267,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>356</v>
@@ -3280,7 +3279,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>356</v>
@@ -3292,7 +3291,7 @@
         <v>446</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -3350,7 +3349,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>356</v>
@@ -3458,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>356</v>
@@ -3496,7 +3495,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>356</v>
@@ -3648,7 +3647,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>356</v>
@@ -3753,7 +3752,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>356</v>
@@ -3782,7 +3781,7 @@
         <v>212</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>356</v>
@@ -3794,7 +3793,7 @@
         <v>366</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>356</v>
@@ -3823,7 +3822,7 @@
         <v>213</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>356</v>
@@ -3835,7 +3834,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>356</v>
@@ -3861,7 +3860,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>356</v>
@@ -3993,7 +3992,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>356</v>
@@ -4031,7 +4030,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>356</v>
@@ -4098,7 +4097,7 @@
         <v>205</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>356</v>
@@ -4174,7 +4173,7 @@
         <v>357</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>357</v>
@@ -4282,7 +4281,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>356</v>
@@ -4472,7 +4471,7 @@
         <v>446</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4498,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>357</v>
@@ -4527,7 +4526,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>356</v>
@@ -4539,7 +4538,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>356</v>
@@ -4568,7 +4567,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>356</v>
@@ -4580,7 +4579,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>356</v>
@@ -4630,7 +4629,7 @@
         <v>446</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4811,7 +4810,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>356</v>
@@ -4840,7 +4839,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>356</v>
@@ -4852,7 +4851,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>356</v>
@@ -4881,7 +4880,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>356</v>
@@ -4893,7 +4892,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>356</v>
@@ -4922,7 +4921,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>356</v>
@@ -4963,7 +4962,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>356</v>
@@ -5004,7 +5003,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>356</v>
@@ -5016,7 +5015,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>356</v>
@@ -5045,7 +5044,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>356</v>
@@ -5057,7 +5056,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>356</v>
@@ -5086,10 +5085,10 @@
         <v>409</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>356</v>
@@ -5127,10 +5126,10 @@
         <v>190</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>356</v>
@@ -5142,7 +5141,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>356</v>
@@ -5192,7 +5191,7 @@
         <v>446</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5227,7 +5226,7 @@
         <v>446</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5285,10 +5284,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>356</v>
@@ -5300,7 +5299,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>356</v>
@@ -5329,10 +5328,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>356</v>
@@ -5344,7 +5343,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>356</v>
@@ -5370,7 +5369,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>356</v>
@@ -5446,7 +5445,7 @@
         <v>149</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I81" s="2">
         <v>86</v>
@@ -5455,7 +5454,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>356</v>
@@ -5493,7 +5492,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>356</v>
@@ -5569,7 +5568,7 @@
         <v>446</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5682,7 +5681,7 @@
         <v>385</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>356</v>
@@ -5694,7 +5693,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>356</v>
@@ -5790,7 +5789,7 @@
         <v>386</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>356</v>
@@ -5828,7 +5827,7 @@
         <v>356</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>357</v>
@@ -5869,7 +5868,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>356</v>
@@ -5898,10 +5897,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>356</v>
@@ -5913,7 +5912,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>356</v>
@@ -5945,7 +5944,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>356</v>
@@ -5957,7 +5956,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>356</v>
@@ -6024,7 +6023,7 @@
         <v>455</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>356</v>
@@ -6068,7 +6067,7 @@
         <v>446</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6097,7 +6096,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>356</v>
@@ -6173,7 +6172,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>356</v>
@@ -6208,7 +6207,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>356</v>
@@ -6296,7 +6295,7 @@
         <v>458</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>169</v>
@@ -6360,7 +6359,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>356</v>
@@ -6401,7 +6400,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>356</v>
@@ -6442,7 +6441,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>356</v>
@@ -6528,7 +6527,7 @@
         <v>446</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6554,7 +6553,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>356</v>
@@ -6590,7 +6589,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>356</v>
@@ -6651,7 +6650,7 @@
         <v>195</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>356</v>
@@ -6663,7 +6662,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>357</v>
@@ -6698,7 +6697,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>356</v>
@@ -6730,7 +6729,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>356</v>
@@ -6862,7 +6861,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>356</v>
@@ -6874,7 +6873,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>356</v>
@@ -7008,7 +7007,7 @@
         <v>71</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>356</v>
@@ -7020,7 +7019,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>356</v>
@@ -7049,7 +7048,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>356</v>
@@ -7061,7 +7060,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>356</v>
@@ -7093,7 +7092,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>356</v>
@@ -7105,7 +7104,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>356</v>
@@ -7175,7 +7174,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>356</v>
@@ -7236,7 +7235,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>356</v>
@@ -7248,7 +7247,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>356</v>
@@ -7277,7 +7276,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>356</v>
@@ -7289,7 +7288,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>356</v>
@@ -7321,7 +7320,7 @@
         <v>444</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>356</v>
@@ -7333,7 +7332,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>356</v>
@@ -7405,7 +7404,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>356</v>
@@ -7446,7 +7445,7 @@
         <v>207</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>356</v>
@@ -7458,7 +7457,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>356</v>
@@ -7487,7 +7486,7 @@
         <v>41</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>356</v>
@@ -7610,7 +7609,7 @@
         <v>446</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -7627,7 +7626,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>356</v>
@@ -7639,7 +7638,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>356</v>
@@ -7700,7 +7699,7 @@
         <v>196</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>356</v>
@@ -7904,7 +7903,7 @@
         <v>413</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>356</v>
@@ -8085,7 +8084,7 @@
         <v>447</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tree transformations, nog improvements
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CCC592-85A0-4446-9D11-97E4B9395BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65414AEC-73AF-490C-AD25-6BD87D6319DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1505,9 +1505,6 @@
     <t>zijn moet er bij maar niet als het Kop is (en dat is nu zo)</t>
   </si>
   <si>
-    <t>//node[@cat="np" and node[@rel="det"] and node[@rel="mod" and @pt="bw" and (not(@special) or @special!="er")] and count(node)=3]</t>
-  </si>
-  <si>
     <t>//node[%Tarsp_OndWBVC%]</t>
   </si>
   <si>
@@ -1906,6 +1903,9 @@
   </si>
   <si>
     <t>//node[@pt="ww" and contains(@lemma,"_") and @rel ="hd" and parent::node[node[@rel="svp" and not(%svpofhww%)]]]</t>
+  </si>
+  <si>
+    <t>//node[(@cat="np" and node[@rel="det"] and node[@rel="mod" and @pt="bw" and (not(@special) or @special!="er")] and count(node)=3) ]</t>
   </si>
 </sst>
 </file>
@@ -2323,15 +2323,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K121" sqref="K121"/>
+      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2395,28 +2394,28 @@
         <v>444</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>562</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>215</v>
       </c>
@@ -2430,13 +2429,13 @@
         <v>194</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>355</v>
@@ -2448,7 +2447,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>355</v>
@@ -2463,7 +2462,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>216</v>
       </c>
@@ -2542,10 +2541,10 @@
         <v>445</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>218</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>219</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>355</v>
@@ -2624,7 +2623,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>220</v>
       </c>
@@ -2635,7 +2634,7 @@
         <v>194</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>355</v>
@@ -2647,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>356</v>
@@ -2659,7 +2658,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>221</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>222</v>
       </c>
@@ -2738,7 +2737,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>223</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>355</v>
@@ -2773,7 +2772,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>224</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>225</v>
       </c>
@@ -2825,7 +2824,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>355</v>
@@ -2837,7 +2836,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>355</v>
@@ -2849,7 +2848,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>226</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>227</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>356</v>
@@ -2922,7 +2921,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>228</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>355</v>
@@ -2957,7 +2956,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>229</v>
       </c>
@@ -2974,7 +2973,7 @@
         <v>355</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>356</v>
@@ -2986,7 +2985,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>230</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>231</v>
       </c>
@@ -3059,7 +3058,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>232</v>
       </c>
@@ -3073,7 +3072,7 @@
         <v>392</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>355</v>
@@ -3085,7 +3084,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>355</v>
@@ -3097,7 +3096,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>233</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>234</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>481</v>
+        <v>602</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>355</v>
@@ -3164,7 +3163,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>235</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>355</v>
@@ -3199,7 +3198,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>236</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>355</v>
@@ -3228,7 +3227,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>355</v>
@@ -3240,7 +3239,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>237</v>
       </c>
@@ -3260,7 +3259,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>355</v>
@@ -3272,7 +3271,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>355</v>
@@ -3284,10 +3283,10 @@
         <v>445</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>238</v>
       </c>
@@ -3319,7 +3318,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>239</v>
       </c>
@@ -3342,7 +3341,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>355</v>
@@ -3357,7 +3356,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>240</v>
       </c>
@@ -3392,7 +3391,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>241</v>
       </c>
@@ -3427,7 +3426,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>242</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>355</v>
@@ -3465,7 +3464,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>243</v>
       </c>
@@ -3488,7 +3487,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>355</v>
@@ -3503,7 +3502,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>244</v>
       </c>
@@ -3538,7 +3537,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>245</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>246</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>355</v>
@@ -3617,7 +3616,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>247</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>355</v>
@@ -3652,7 +3651,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>248</v>
       </c>
@@ -3687,7 +3686,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>249</v>
       </c>
@@ -3722,7 +3721,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>250</v>
       </c>
@@ -3745,7 +3744,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>355</v>
@@ -3757,7 +3756,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>251</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>211</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>355</v>
@@ -3786,7 +3785,7 @@
         <v>365</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>355</v>
@@ -3798,7 +3797,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>252</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>212</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>355</v>
@@ -3827,7 +3826,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>355</v>
@@ -3839,7 +3838,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>253</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>355</v>
@@ -3865,7 +3864,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>355</v>
@@ -3880,7 +3879,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>254</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>255</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>256</v>
       </c>
@@ -3985,7 +3984,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>355</v>
@@ -4000,7 +3999,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>257</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>355</v>
@@ -4035,7 +4034,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>258</v>
       </c>
@@ -4058,7 +4057,7 @@
         <v>6</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>355</v>
@@ -4070,7 +4069,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>259</v>
       </c>
@@ -4090,7 +4089,7 @@
         <v>204</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>355</v>
@@ -4102,7 +4101,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>355</v>
@@ -4114,7 +4113,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>260</v>
       </c>
@@ -4137,7 +4136,7 @@
         <v>6</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>355</v>
@@ -4152,7 +4151,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>261</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>356</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>356</v>
@@ -4181,7 +4180,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>262</v>
       </c>
@@ -4216,7 +4215,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>263</v>
       </c>
@@ -4251,7 +4250,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>264</v>
       </c>
@@ -4274,7 +4273,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>355</v>
@@ -4286,7 +4285,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>265</v>
       </c>
@@ -4324,7 +4323,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>266</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>355</v>
@@ -4359,7 +4358,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>267</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>6</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>355</v>
@@ -4397,7 +4396,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>268</v>
       </c>
@@ -4464,10 +4463,10 @@
         <v>445</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>270</v>
       </c>
@@ -4490,7 +4489,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>356</v>
@@ -4502,7 +4501,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>271</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>355</v>
@@ -4531,7 +4530,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>355</v>
@@ -4543,7 +4542,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>272</v>
       </c>
@@ -4560,7 +4559,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>355</v>
@@ -4572,7 +4571,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>355</v>
@@ -4622,10 +4621,10 @@
         <v>445</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>274</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>275</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>276</v>
       </c>
@@ -4739,7 +4738,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>277</v>
       </c>
@@ -4774,7 +4773,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>278</v>
       </c>
@@ -4803,7 +4802,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>355</v>
@@ -4815,7 +4814,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>279</v>
       </c>
@@ -4832,7 +4831,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>355</v>
@@ -4844,7 +4843,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>355</v>
@@ -4856,7 +4855,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>280</v>
       </c>
@@ -4873,7 +4872,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>355</v>
@@ -4885,7 +4884,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>355</v>
@@ -4897,7 +4896,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>281</v>
       </c>
@@ -4914,7 +4913,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>355</v>
@@ -4926,7 +4925,7 @@
         <v>4</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>355</v>
@@ -4938,7 +4937,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>282</v>
       </c>
@@ -4955,7 +4954,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>355</v>
@@ -4967,7 +4966,7 @@
         <v>4</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>355</v>
@@ -4979,7 +4978,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>283</v>
       </c>
@@ -4996,7 +4995,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>355</v>
@@ -5008,7 +5007,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>355</v>
@@ -5020,7 +5019,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>284</v>
       </c>
@@ -5037,7 +5036,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>355</v>
@@ -5049,7 +5048,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>355</v>
@@ -5061,7 +5060,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>285</v>
       </c>
@@ -5078,10 +5077,10 @@
         <v>408</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>355</v>
@@ -5102,7 +5101,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>286</v>
       </c>
@@ -5119,10 +5118,10 @@
         <v>189</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>355</v>
@@ -5134,7 +5133,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>355</v>
@@ -5184,7 +5183,7 @@
         <v>445</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5219,10 +5218,10 @@
         <v>445</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>289</v>
       </c>
@@ -5260,7 +5259,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>290</v>
       </c>
@@ -5277,10 +5276,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>355</v>
@@ -5292,7 +5291,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>355</v>
@@ -5304,7 +5303,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>291</v>
       </c>
@@ -5321,10 +5320,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>355</v>
@@ -5336,7 +5335,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>355</v>
@@ -5348,7 +5347,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>292</v>
       </c>
@@ -5362,7 +5361,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>355</v>
@@ -5386,7 +5385,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>293</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>294</v>
       </c>
@@ -5438,7 +5437,7 @@
         <v>149</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I81" s="2">
         <v>86</v>
@@ -5447,7 +5446,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>355</v>
@@ -5459,7 +5458,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>295</v>
       </c>
@@ -5485,7 +5484,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>355</v>
@@ -5497,7 +5496,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>296</v>
       </c>
@@ -5561,10 +5560,10 @@
         <v>445</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>298</v>
       </c>
@@ -5596,7 +5595,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>299</v>
       </c>
@@ -5628,7 +5627,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>300</v>
       </c>
@@ -5660,7 +5659,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>301</v>
       </c>
@@ -5674,7 +5673,7 @@
         <v>384</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>355</v>
@@ -5686,7 +5685,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>355</v>
@@ -5698,7 +5697,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>302</v>
       </c>
@@ -5721,7 +5720,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>355</v>
@@ -5733,7 +5732,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>303</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>389</v>
       </c>
@@ -5782,7 +5781,7 @@
         <v>385</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>355</v>
@@ -5806,7 +5805,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>304</v>
       </c>
@@ -5820,7 +5819,7 @@
         <v>355</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>356</v>
@@ -5832,7 +5831,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>305</v>
       </c>
@@ -5861,7 +5860,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>355</v>
@@ -5873,7 +5872,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>306</v>
       </c>
@@ -5890,10 +5889,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>355</v>
@@ -5905,7 +5904,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>355</v>
@@ -5920,7 +5919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>307</v>
       </c>
@@ -5937,7 +5936,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>355</v>
@@ -5949,7 +5948,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>355</v>
@@ -5961,7 +5960,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>308</v>
       </c>
@@ -5996,7 +5995,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>309</v>
       </c>
@@ -6016,7 +6015,7 @@
         <v>454</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>355</v>
@@ -6060,10 +6059,10 @@
         <v>445</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="99" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>311</v>
       </c>
@@ -6089,7 +6088,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>355</v>
@@ -6104,7 +6103,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="100" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>312</v>
       </c>
@@ -6142,7 +6141,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="101" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>313</v>
       </c>
@@ -6165,7 +6164,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>355</v>
@@ -6177,7 +6176,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="102" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>314</v>
       </c>
@@ -6200,7 +6199,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>355</v>
@@ -6212,7 +6211,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="103" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>315</v>
       </c>
@@ -6288,13 +6287,13 @@
         <v>457</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="105" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>317</v>
       </c>
@@ -6323,7 +6322,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="106" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>318</v>
       </c>
@@ -6352,7 +6351,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>355</v>
@@ -6367,7 +6366,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>319</v>
       </c>
@@ -6393,7 +6392,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>355</v>
@@ -6408,7 +6407,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="108" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>320</v>
       </c>
@@ -6434,7 +6433,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>355</v>
@@ -6452,7 +6451,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>321</v>
       </c>
@@ -6475,7 +6474,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>355</v>
@@ -6520,10 +6519,10 @@
         <v>445</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>323</v>
       </c>
@@ -6546,7 +6545,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>355</v>
@@ -6558,7 +6557,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>324</v>
       </c>
@@ -6582,7 +6581,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>355</v>
@@ -6594,10 +6593,10 @@
         <v>445</v>
       </c>
       <c r="U112" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="113" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>325</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="114" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>326</v>
       </c>
@@ -6643,7 +6642,7 @@
         <v>194</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>355</v>
@@ -6655,7 +6654,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>356</v>
@@ -6667,7 +6666,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>327</v>
       </c>
@@ -6690,7 +6689,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>355</v>
@@ -6702,10 +6701,10 @@
         <v>445</v>
       </c>
       <c r="U115" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="116" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>328</v>
       </c>
@@ -6722,7 +6721,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>355</v>
@@ -6746,7 +6745,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="117" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>329</v>
       </c>
@@ -6774,7 +6773,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="118" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>330</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="119" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>331</v>
       </c>
@@ -6837,7 +6836,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="120" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>332</v>
       </c>
@@ -6854,7 +6853,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>355</v>
@@ -6866,7 +6865,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>355</v>
@@ -6878,7 +6877,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="121" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>333</v>
       </c>
@@ -6901,7 +6900,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>355</v>
@@ -6913,7 +6912,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="122" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>334</v>
       </c>
@@ -6936,7 +6935,7 @@
         <v>3</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>356</v>
@@ -6948,7 +6947,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>335</v>
       </c>
@@ -6983,7 +6982,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="124" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>336</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>71</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>355</v>
@@ -7012,7 +7011,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>355</v>
@@ -7024,7 +7023,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="125" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>337</v>
       </c>
@@ -7041,7 +7040,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>355</v>
@@ -7053,7 +7052,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>355</v>
@@ -7068,7 +7067,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="126" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>338</v>
       </c>
@@ -7085,7 +7084,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>355</v>
@@ -7097,7 +7096,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>355</v>
@@ -7109,7 +7108,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>339</v>
       </c>
@@ -7144,7 +7143,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="128" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>340</v>
       </c>
@@ -7167,7 +7166,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>355</v>
@@ -7179,7 +7178,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="129" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>341</v>
       </c>
@@ -7211,7 +7210,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="130" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>342</v>
       </c>
@@ -7228,7 +7227,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>355</v>
@@ -7240,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>355</v>
@@ -7252,7 +7251,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="131" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>343</v>
       </c>
@@ -7269,7 +7268,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>355</v>
@@ -7281,7 +7280,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>355</v>
@@ -7293,7 +7292,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="132" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>344</v>
       </c>
@@ -7313,7 +7312,7 @@
         <v>443</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>355</v>
@@ -7325,7 +7324,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>355</v>
@@ -7340,7 +7339,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="133" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>345</v>
       </c>
@@ -7379,7 +7378,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>346</v>
       </c>
@@ -7397,7 +7396,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>355</v>
@@ -7418,7 +7417,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="135" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>347</v>
       </c>
@@ -7438,7 +7437,7 @@
         <v>206</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>355</v>
@@ -7450,7 +7449,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>355</v>
@@ -7462,7 +7461,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="136" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>348</v>
       </c>
@@ -7479,7 +7478,7 @@
         <v>41</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>355</v>
@@ -7500,7 +7499,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="137" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>349</v>
       </c>
@@ -7535,7 +7534,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="138" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>350</v>
       </c>
@@ -7602,10 +7601,10 @@
         <v>445</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="140" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>352</v>
       </c>
@@ -7619,7 +7618,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>355</v>
@@ -7631,7 +7630,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>355</v>
@@ -7643,7 +7642,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>353</v>
       </c>
@@ -7681,7 +7680,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="142" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>362</v>
       </c>
@@ -7692,7 +7691,7 @@
         <v>195</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>355</v>
@@ -7716,7 +7715,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="143" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>393</v>
       </c>
@@ -7751,7 +7750,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="144" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>394</v>
       </c>
@@ -7783,7 +7782,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="145" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>395</v>
       </c>
@@ -7815,7 +7814,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="146" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>403</v>
       </c>
@@ -7850,7 +7849,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="147" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>459</v>
       </c>
@@ -7882,7 +7881,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="148" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>407</v>
       </c>
@@ -7896,7 +7895,7 @@
         <v>412</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>355</v>
@@ -7917,7 +7916,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>447</v>
       </c>
@@ -7949,7 +7948,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="150" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>461</v>
       </c>
@@ -7981,7 +7980,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="151" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>462</v>
       </c>
@@ -8013,7 +8012,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="152" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>463</v>
       </c>
@@ -8077,10 +8076,10 @@
         <v>446</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="154" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>469</v>
       </c>
@@ -8109,21 +8108,21 @@
         <v>446</v>
       </c>
     </row>
-    <row r="155" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H155" s="2" t="s">
         <v>355</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>355</v>
@@ -8135,18 +8134,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="156" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V156" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="7"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:V156" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N146">
     <sortCondition ref="E2:E146"/>
     <sortCondition ref="I2:I146"/>

</xml_diff>

<commit_message>
spellingcorrection updates, evaluation updates
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D3AE22-679B-4B57-8D62-084CE6FFA9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4E6453-76C7-42DF-8E67-F72DE273DC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="602">
   <si>
     <t>Item</t>
   </si>
@@ -1854,9 +1854,6 @@
   <si>
     <t>//node[@pt="ww" and @pvagr="met-t" and not(%Tarsp_Kop%) and
 not(%Tarsp_hww% or %hebbenwordenzijn%  ) ]</t>
-  </si>
-  <si>
-    <t>99</t>
   </si>
   <si>
     <t>//node[node[(@lemma="een" or @lemma="'n") and @pt="lid"] and node[@pt="n" and @rel="hd"] and count(node)=2 ]</t>
@@ -2323,11 +2320,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
+      <selection pane="bottomRight" activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2757,7 +2754,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>355</v>
@@ -3081,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>355</v>
@@ -3148,7 +3145,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>355</v>
@@ -3268,7 +3265,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>355</v>
@@ -3446,7 +3443,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>355</v>
@@ -3601,7 +3598,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>355</v>
@@ -3823,7 +3820,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>355</v>
@@ -4270,7 +4267,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>355</v>
@@ -5434,7 +5431,7 @@
         <v>149</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>587</v>
+        <v>355</v>
       </c>
       <c r="I81" s="2">
         <v>86</v>
@@ -5682,7 +5679,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>355</v>
@@ -5886,7 +5883,7 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>573</v>
@@ -6085,7 +6082,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>355</v>
@@ -6686,7 +6683,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>355</v>
@@ -6897,7 +6894,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>355</v>
@@ -7446,7 +7443,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>355</v>
@@ -7627,7 +7624,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>355</v>

</xml_diff>

<commit_message>
changes for mwequery and sasta self assessment
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A129E9F-434C-45A0-8031-5F608851A08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB364E95-FF1E-457B-9629-64E956125833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2323,11 +2323,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="N19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="P31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="R157" sqref="R157"/>
+      <selection pane="bottomRight" activeCell="R163" sqref="R163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
SAS updates, ASTA unaligned annotation
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB364E95-FF1E-457B-9629-64E956125833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BC5641-C9D1-46D4-B7F2-0609150B9B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="604">
   <si>
     <t>Item</t>
   </si>
@@ -1903,6 +1903,9 @@
   </si>
   <si>
     <t>tarsp2005,tarsp2017</t>
+  </si>
+  <si>
+    <t>WOndX</t>
   </si>
 </sst>
 </file>
@@ -2024,9 +2027,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2064,7 +2067,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2170,7 +2173,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2312,7 +2315,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2323,11 +2326,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="R163" sqref="R163"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7001,6 +7004,9 @@
       <c r="E124" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="F124" s="2" t="s">
+        <v>603</v>
+      </c>
       <c r="G124" s="2" t="s">
         <v>575</v>
       </c>

</xml_diff>

<commit_message>
Updates for SASTASelf Assessment and various small improvements of [C[2~
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BC5641-C9D1-46D4-B7F2-0609150B9B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409BD3A1-5ECE-492E-8D4F-FDAC46CF52D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="609">
   <si>
     <t>Item</t>
   </si>
@@ -1565,12 +1565,6 @@
   </si>
   <si>
     <t>//node[%Tarsp_HwwZ%]</t>
-  </si>
-  <si>
-    <t>//node[node[@rel="hd" and @pt="vz"] and 
-       node[@rel="obj1" and 
-            ( (@pt="vz" or @pt="bw") or 
-              (%Rpronoun% and @begin=../node[@rel="hd"]/@end)) ]]</t>
   </si>
   <si>
     <t>vu nee/ja, vu ja/nee,V.U. Ja/nee, nee, ja</t>
@@ -1906,6 +1900,27 @@
   </si>
   <si>
     <t>WOndX</t>
+  </si>
+  <si>
+    <t>//node[node[@rel="hd" and @pt="vz"] and 
+       node[@rel="obj1" and 
+            ( (@pt="vz" or @pt="bw") or 
+              (%Rpronoun% and @begin&gt;=../node[@rel="hd"]/@end)) ]]</t>
+  </si>
+  <si>
+    <t>T166</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>//node[ @lemma="niets" or @lemma="niks" or @lemma="zelf"]</t>
+  </si>
+  <si>
+    <t>tarsp2017,auris</t>
+  </si>
+  <si>
+    <t>taalmaat is veranderd in 2017; vgl T085</t>
   </si>
 </sst>
 </file>
@@ -2326,11 +2341,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="N141" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="U157" sqref="U157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2394,22 +2409,22 @@
         <v>443</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>559</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2429,13 +2444,13 @@
         <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>354</v>
@@ -2447,7 +2462,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>354</v>
@@ -2541,7 +2556,7 @@
         <v>444</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2605,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>354</v>
@@ -2634,7 +2649,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>354</v>
@@ -2646,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>355</v>
@@ -2760,7 +2775,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>354</v>
@@ -2824,7 +2839,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>354</v>
@@ -2836,7 +2851,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>354</v>
@@ -2944,7 +2959,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>354</v>
@@ -3072,7 +3087,7 @@
         <v>391</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>354</v>
@@ -3084,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>354</v>
@@ -3151,7 +3166,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>354</v>
@@ -3215,7 +3230,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>354</v>
@@ -3227,7 +3242,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>354</v>
@@ -3259,7 +3274,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>354</v>
@@ -3271,7 +3286,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>354</v>
@@ -3283,7 +3298,7 @@
         <v>444</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -3341,7 +3356,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>354</v>
@@ -3449,7 +3464,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>354</v>
@@ -3487,7 +3502,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>354</v>
@@ -3537,7 +3552,7 @@
         <v>444</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -3607,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>354</v>
@@ -3619,7 +3634,7 @@
         <v>444</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3645,7 +3660,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>354</v>
@@ -3750,7 +3765,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>354</v>
@@ -3779,7 +3794,7 @@
         <v>210</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>354</v>
@@ -3791,7 +3806,7 @@
         <v>364</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>354</v>
@@ -3820,7 +3835,7 @@
         <v>211</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>354</v>
@@ -3832,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>354</v>
@@ -3858,7 +3873,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>354</v>
@@ -3990,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>354</v>
@@ -4028,7 +4043,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>354</v>
@@ -4095,7 +4110,7 @@
         <v>203</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>354</v>
@@ -4171,7 +4186,7 @@
         <v>355</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>355</v>
@@ -4279,7 +4294,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>354</v>
@@ -4317,7 +4332,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>354</v>
@@ -4469,7 +4484,7 @@
         <v>444</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4495,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>355</v>
@@ -4524,7 +4539,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>354</v>
@@ -4536,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>354</v>
@@ -4565,7 +4580,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>354</v>
@@ -4577,7 +4592,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>354</v>
@@ -4627,7 +4642,7 @@
         <v>444</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4808,7 +4823,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>354</v>
@@ -4837,7 +4852,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>354</v>
@@ -4849,7 +4864,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>354</v>
@@ -4878,7 +4893,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>354</v>
@@ -4890,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>354</v>
@@ -4919,7 +4934,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>354</v>
@@ -4960,7 +4975,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>354</v>
@@ -5001,7 +5016,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>354</v>
@@ -5013,7 +5028,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>354</v>
@@ -5042,7 +5057,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>354</v>
@@ -5054,7 +5069,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>354</v>
@@ -5083,10 +5098,10 @@
         <v>407</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>354</v>
@@ -5124,10 +5139,10 @@
         <v>188</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>354</v>
@@ -5139,7 +5154,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>354</v>
@@ -5189,7 +5204,7 @@
         <v>444</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5224,7 +5239,7 @@
         <v>444</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5282,10 +5297,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>354</v>
@@ -5297,7 +5312,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>354</v>
@@ -5326,10 +5341,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>354</v>
@@ -5341,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>354</v>
@@ -5367,7 +5382,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>354</v>
@@ -5389,6 +5404,9 @@
       </c>
       <c r="N79" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="R79" s="2" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
@@ -5452,7 +5470,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>354</v>
@@ -5490,7 +5508,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>354</v>
@@ -5566,7 +5584,7 @@
         <v>444</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5679,7 +5697,7 @@
         <v>383</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>354</v>
@@ -5691,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>354</v>
@@ -5787,7 +5805,7 @@
         <v>384</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>354</v>
@@ -5825,7 +5843,7 @@
         <v>354</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>355</v>
@@ -5866,7 +5884,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>354</v>
@@ -5895,10 +5913,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>354</v>
@@ -5910,7 +5928,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>354</v>
@@ -5942,7 +5960,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>354</v>
@@ -5954,7 +5972,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>354</v>
@@ -6021,7 +6039,7 @@
         <v>453</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>354</v>
@@ -6065,7 +6083,7 @@
         <v>444</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6094,7 +6112,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>354</v>
@@ -6170,7 +6188,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>354</v>
@@ -6205,7 +6223,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>354</v>
@@ -6293,7 +6311,7 @@
         <v>456</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>167</v>
@@ -6357,7 +6375,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>354</v>
@@ -6398,7 +6416,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>354</v>
@@ -6439,7 +6457,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>354</v>
@@ -6480,7 +6498,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>499</v>
+        <v>603</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>354</v>
@@ -6525,7 +6543,7 @@
         <v>444</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6551,7 +6569,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>354</v>
@@ -6587,7 +6605,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>354</v>
@@ -6648,7 +6666,7 @@
         <v>193</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>354</v>
@@ -6660,7 +6678,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>355</v>
@@ -6695,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>354</v>
@@ -6727,7 +6745,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>354</v>
@@ -6859,7 +6877,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>354</v>
@@ -6871,7 +6889,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>354</v>
@@ -6906,7 +6924,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>354</v>
@@ -7005,10 +7023,10 @@
         <v>71</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>354</v>
@@ -7020,7 +7038,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>354</v>
@@ -7049,7 +7067,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>354</v>
@@ -7061,7 +7079,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>354</v>
@@ -7093,7 +7111,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>354</v>
@@ -7105,7 +7123,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>354</v>
@@ -7175,7 +7193,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>354</v>
@@ -7236,7 +7254,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>354</v>
@@ -7248,7 +7266,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>354</v>
@@ -7277,7 +7295,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>354</v>
@@ -7289,7 +7307,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>354</v>
@@ -7321,7 +7339,7 @@
         <v>442</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>354</v>
@@ -7333,7 +7351,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>354</v>
@@ -7405,7 +7423,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>354</v>
@@ -7446,7 +7464,7 @@
         <v>205</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>354</v>
@@ -7458,7 +7476,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>354</v>
@@ -7487,7 +7505,7 @@
         <v>41</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>354</v>
@@ -7610,7 +7628,7 @@
         <v>444</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -7627,7 +7645,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>354</v>
@@ -7639,7 +7657,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>354</v>
@@ -7700,7 +7718,7 @@
         <v>194</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>354</v>
@@ -7904,7 +7922,7 @@
         <v>411</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>354</v>
@@ -8085,7 +8103,7 @@
         <v>445</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">
@@ -8144,8 +8162,48 @@
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="K156" s="3"/>
-      <c r="L156" s="3"/>
+      <c r="A156" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I156" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="J156" s="2">
+        <v>6</v>
+      </c>
+      <c r="K156" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="R156" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="U156" s="2" t="s">
+        <v>608</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:V156" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
various small improvements for TARSP
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409BD3A1-5ECE-492E-8D4F-FDAC46CF52D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1097ED3D-B6FA-4B19-B294-55EC241B6887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1847,9 +1847,6 @@
 not(%Tarsp_hww% or %hebbenwordenzijn%  ) ]</t>
   </si>
   <si>
-    <t>//node[node[(@lemma="een" or @lemma="'n") and @pt="lid"] and node[@pt="n" and @rel="hd"] and count(node)=2 ]</t>
-  </si>
-  <si>
     <t>//node[%Tarsp_BX%]</t>
   </si>
   <si>
@@ -1921,6 +1918,9 @@
   </si>
   <si>
     <t>taalmaat is veranderd in 2017; vgl T085</t>
+  </si>
+  <si>
+    <t>//node[node[(@lemma="een" or @lemma="'n") and @pt="lid"] and node[(@pt="n" or (@pt="adj" and @positie="nom")) and @rel="hd"] and count(node)=2 ]</t>
   </si>
 </sst>
 </file>
@@ -2341,11 +2341,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="N141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="U157" sqref="U157"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2775,7 +2775,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>354</v>
@@ -3099,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>354</v>
@@ -3166,7 +3166,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>354</v>
@@ -3286,7 +3286,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>354</v>
@@ -3464,7 +3464,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>585</v>
+        <v>608</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>354</v>
@@ -3622,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>354</v>
@@ -3634,7 +3634,7 @@
         <v>444</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3847,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>354</v>
@@ -4294,7 +4294,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>354</v>
@@ -4332,7 +4332,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>354</v>
@@ -5709,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>354</v>
@@ -5913,7 +5913,7 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>571</v>
@@ -6112,7 +6112,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>354</v>
@@ -6498,7 +6498,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>354</v>
@@ -6713,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>354</v>
@@ -6924,7 +6924,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>354</v>
@@ -7023,7 +7023,7 @@
         <v>71</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>574</v>
@@ -7476,7 +7476,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>354</v>
@@ -7657,7 +7657,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>354</v>
@@ -8163,7 +8163,7 @@
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>125</v>
@@ -8181,28 +8181,28 @@
         <v>354</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J156" s="2">
         <v>6</v>
       </c>
       <c r="K156" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="R156" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="L156" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M156" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="N156" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="R156" s="2" t="s">
+      <c r="U156" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="U156" s="2" t="s">
-        <v>608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>